<commit_message>
add periodicity to the file && add img showcasing file is generated and made some changes to it by adding some columns
</commit_message>
<xml_diff>
--- a/DAV Proforma Acc Analy.xlsx
+++ b/DAV Proforma Acc Analy.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,25 +520,30 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>Periodicity</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Attribution Gross</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Attribution Net</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Opening Allocation</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Closing Allocation</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Investment Performance</t>
         </is>
@@ -592,19 +597,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
         <v>2.119265104055602e-05</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>2.108889938052946e-05</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>0.005174539139199182</v>
       </c>
-      <c r="U2" t="n">
+      <c r="V2" t="n">
         <v>0.005189781105213061</v>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>0.004095563</v>
       </c>
     </row>
@@ -656,19 +666,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R3" t="n">
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
         <v>2.909538323649109e-05</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>2.899163157646453e-05</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>0.005230934441045491</v>
       </c>
-      <c r="U3" t="n">
+      <c r="V3" t="n">
         <v>0.005254005498550999</v>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>0.005562177000000001</v>
       </c>
     </row>
@@ -720,19 +735,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R4" t="n">
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
         <v>-3.49666242881802e-06</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>-3.600414088844581e-06</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>0.005115617128245146</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>0.005106265541055268</v>
       </c>
-      <c r="V4" t="n">
+      <c r="W4" t="n">
         <v>-0.0006835270000000001</v>
       </c>
     </row>
@@ -784,19 +804,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R5" t="n">
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
         <v>2.123826364885281e-05</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>2.113451198882625e-05</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>0.005195238201540551</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>0.005210502021232976</v>
       </c>
-      <c r="V5" t="n">
+      <c r="W5" t="n">
         <v>0.004088025</v>
       </c>
     </row>
@@ -848,19 +873,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
         <v>2.755475023853125e-05</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>2.745099857850469e-05</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>0.005093760846829241</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>0.005115450141099162</v>
       </c>
-      <c r="V6" t="n">
+      <c r="W6" t="n">
         <v>0.005409509999999999</v>
       </c>
     </row>
@@ -912,19 +942,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
         <v>-2.070168479317965e-06</v>
       </c>
-      <c r="S7" t="n">
+      <c r="T7" t="n">
         <v>-2.173920139344526e-06</v>
       </c>
-      <c r="T7" t="n">
+      <c r="U7" t="n">
         <v>0.005337583661923733</v>
       </c>
-      <c r="U7" t="n">
+      <c r="V7" t="n">
         <v>0.005329402716072358</v>
       </c>
-      <c r="V7" t="n">
+      <c r="W7" t="n">
         <v>-0.0003878475</v>
       </c>
     </row>
@@ -976,19 +1011,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
         <v>-1.940408807975866e-05</v>
       </c>
-      <c r="S8" t="n">
+      <c r="T8" t="n">
         <v>-1.950783973978522e-05</v>
       </c>
-      <c r="T8" t="n">
+      <c r="U8" t="n">
         <v>0.005392179840708177</v>
       </c>
-      <c r="U8" t="n">
+      <c r="V8" t="n">
         <v>0.005366622298694765</v>
       </c>
-      <c r="V8" t="n">
+      <c r="W8" t="n">
         <v>-0.003598561</v>
       </c>
     </row>
@@ -1040,19 +1080,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
         <v>-9.976623552509027e-06</v>
       </c>
-      <c r="S9" t="n">
+      <c r="T9" t="n">
         <v>-1.008037521253559e-05</v>
       </c>
-      <c r="T9" t="n">
+      <c r="U9" t="n">
         <v>0.005244379073264815</v>
       </c>
-      <c r="U9" t="n">
+      <c r="V9" t="n">
         <v>0.005228407475079547</v>
       </c>
-      <c r="V9" t="n">
+      <c r="W9" t="n">
         <v>-0.001902346</v>
       </c>
     </row>
@@ -1104,19 +1149,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R10" t="n">
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
         <v>-1.749415581952579e-05</v>
       </c>
-      <c r="S10" t="n">
+      <c r="T10" t="n">
         <v>-1.759790747955235e-05</v>
       </c>
-      <c r="T10" t="n">
+      <c r="U10" t="n">
         <v>0.005271936191132592</v>
       </c>
-      <c r="U10" t="n">
+      <c r="V10" t="n">
         <v>0.005248424109291207</v>
       </c>
-      <c r="V10" t="n">
+      <c r="W10" t="n">
         <v>-0.003318355</v>
       </c>
     </row>
@@ -1168,19 +1218,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R11" t="n">
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
         <v>-1.387199700328407e-05</v>
       </c>
-      <c r="S11" t="n">
+      <c r="T11" t="n">
         <v>-1.397574866331063e-05</v>
       </c>
-      <c r="T11" t="n">
+      <c r="U11" t="n">
         <v>0.005165307758234378</v>
       </c>
-      <c r="U11" t="n">
+      <c r="V11" t="n">
         <v>0.005145535808560743</v>
       </c>
-      <c r="V11" t="n">
+      <c r="W11" t="n">
         <v>-0.002685609</v>
       </c>
     </row>
@@ -1232,19 +1287,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R12" t="n">
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
         <v>-4.709926678570521e-06</v>
       </c>
-      <c r="S12" t="n">
+      <c r="T12" t="n">
         <v>-4.813678338597081e-06</v>
       </c>
-      <c r="T12" t="n">
+      <c r="U12" t="n">
         <v>0.005268524048189424</v>
       </c>
-      <c r="U12" t="n">
+      <c r="V12" t="n">
         <v>0.005257785461614488</v>
       </c>
-      <c r="V12" t="n">
+      <c r="W12" t="n">
         <v>-0.0008939746</v>
       </c>
     </row>
@@ -1310,19 +1370,24 @@
           <t>02/03/2021</t>
         </is>
       </c>
-      <c r="R13" t="n">
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
         <v>-1.182319737245871e-05</v>
       </c>
-      <c r="S13" t="n">
+      <c r="T13" t="n">
         <v>-1.192694903248527e-05</v>
       </c>
-      <c r="T13" t="n">
+      <c r="U13" t="n">
         <v>0.005093258739147339</v>
       </c>
-      <c r="U13" t="n">
+      <c r="V13" t="n">
         <v>0.005075615760536505</v>
       </c>
-      <c r="V13" t="n">
+      <c r="W13" t="n">
         <v>-0.002321342381761275</v>
       </c>
     </row>
@@ -1374,19 +1439,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R14" t="n">
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
         <v>4.873944153466173e-06</v>
       </c>
-      <c r="S14" t="n">
+      <c r="T14" t="n">
         <v>4.770192493439613e-06</v>
       </c>
-      <c r="T14" t="n">
+      <c r="U14" t="n">
         <v>0.005200498538120522</v>
       </c>
-      <c r="U14" t="n">
+      <c r="V14" t="n">
         <v>0.005199410755737846</v>
       </c>
-      <c r="V14" t="n">
+      <c r="W14" t="n">
         <v>0.0009372070999999999</v>
       </c>
     </row>
@@ -1438,19 +1508,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R15" t="n">
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
         <v>8.608351373399145e-05</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>8.597976207396488e-05</v>
       </c>
-      <c r="T15" t="n">
+      <c r="U15" t="n">
         <v>0.005480649077310507</v>
       </c>
-      <c r="U15" t="n">
+      <c r="V15" t="n">
         <v>0.00556035699784331</v>
       </c>
-      <c r="V15" t="n">
+      <c r="W15" t="n">
         <v>0.01570681</v>
       </c>
     </row>
@@ -1502,19 +1577,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R16" t="n">
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
         <v>2.042675073927907e-05</v>
       </c>
-      <c r="S16" t="n">
+      <c r="T16" t="n">
         <v>2.03229990792525e-05</v>
       </c>
-      <c r="T16" t="n">
+      <c r="U16" t="n">
         <v>0.005154269371994643</v>
       </c>
-      <c r="U16" t="n">
+      <c r="V16" t="n">
         <v>0.00516876952991152</v>
       </c>
-      <c r="V16" t="n">
+      <c r="W16" t="n">
         <v>0.003963073961610615</v>
       </c>
     </row>
@@ -1566,19 +1646,24 @@
           <t>02/02/2021</t>
         </is>
       </c>
-      <c r="R17" t="n">
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
         <v>0.000111551947782771</v>
       </c>
-      <c r="S17" t="n">
+      <c r="T17" t="n">
         <v>0.0001114481961227444</v>
       </c>
-      <c r="T17" t="n">
+      <c r="U17" t="n">
         <v>0.005144395617834251</v>
       </c>
-      <c r="U17" t="n">
+      <c r="V17" t="n">
         <v>0.005249927915307422</v>
       </c>
-      <c r="V17" t="n">
+      <c r="W17" t="n">
         <v>0.02168416973921097</v>
       </c>
     </row>
@@ -1644,19 +1729,24 @@
           <t>02/03/2021</t>
         </is>
       </c>
-      <c r="R18" t="n">
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
         <v>0</v>
       </c>
-      <c r="S18" t="n">
+      <c r="T18" t="n">
         <v>-1.037516600265604e-07</v>
       </c>
-      <c r="T18" t="n">
+      <c r="U18" t="n">
         <v>0.005084848499272712</v>
       </c>
-      <c r="U18" t="n">
+      <c r="V18" t="n">
         <v>0.005079024809165308</v>
       </c>
-      <c r="V18" t="n">
+      <c r="W18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1708,19 +1798,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R19" t="n">
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
         <v>0.0001569015430658485</v>
       </c>
-      <c r="S19" t="n">
+      <c r="T19" t="n">
         <v>0.0001567977914058219</v>
       </c>
-      <c r="T19" t="n">
+      <c r="U19" t="n">
         <v>0.005117737798983247</v>
       </c>
-      <c r="U19" t="n">
+      <c r="V19" t="n">
         <v>0.005268598283999714</v>
       </c>
-      <c r="V19" t="n">
+      <c r="W19" t="n">
         <v>0.03065837860959202</v>
       </c>
     </row>
@@ -1772,19 +1867,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R20" t="n">
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
         <v>2.355563315332659e-05</v>
       </c>
-      <c r="S20" t="n">
+      <c r="T20" t="n">
         <v>2.345188149330003e-05</v>
       </c>
-      <c r="T20" t="n">
+      <c r="U20" t="n">
         <v>0.005161642023061436</v>
       </c>
-      <c r="U20" t="n">
+      <c r="V20" t="n">
         <v>0.005179259035958967</v>
       </c>
-      <c r="V20" t="n">
+      <c r="W20" t="n">
         <v>0.004563592951251479</v>
       </c>
     </row>
@@ -1836,19 +1936,24 @@
           <t>02/04/2021</t>
         </is>
       </c>
-      <c r="R21" t="n">
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Daily</t>
+        </is>
+      </c>
+      <c r="S21" t="n">
         <v>2.123826364885281e-05</v>
       </c>
-      <c r="S21" t="n">
+      <c r="T21" t="n">
         <v>2.113451198882625e-05</v>
       </c>
-      <c r="T21" t="n">
+      <c r="U21" t="n">
         <v>0.005195238201540551</v>
       </c>
-      <c r="U21" t="n">
+      <c r="V21" t="n">
         <v>0.005210502021232976</v>
       </c>
-      <c r="V21" t="n">
+      <c r="W21" t="n">
         <v>0.004088025</v>
       </c>
     </row>

</xml_diff>